<commit_message>
Fix formatting issue in insertDuracionEnCampos method in ProductoController
</commit_message>
<xml_diff>
--- a/storage/app/public/plantillas/Prueba certificado 7.xlsx
+++ b/storage/app/public/plantillas/Prueba certificado 7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIGUEL\Desktop\backend-kyrema\storage\app\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEFDC43-A733-472A-9DB9-433CA4CC0F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A64681-B196-48A5-8915-96370A3288FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -318,6 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,7 +358,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,18 +509,18 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>470353</xdr:colOff>
+      <xdr:colOff>385686</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>60476</xdr:rowOff>
+      <xdr:rowOff>36286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>132140</xdr:colOff>
+      <xdr:colOff>47473</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>146654</xdr:rowOff>
+      <xdr:rowOff>122464</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -543,7 +543,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7715401" y="60476"/>
+          <a:off x="7630734" y="36286"/>
           <a:ext cx="2080834" cy="630464"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="P220" sqref="P220"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="63" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -897,13 +897,13 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
       <c r="N4" s="18"/>
       <c r="O4" t="s">
         <v>30</v>
@@ -927,16 +927,16 @@
       <c r="O5" s="18"/>
     </row>
     <row r="6" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
@@ -946,14 +946,14 @@
       <c r="O6" s="18"/>
     </row>
     <row r="7" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
@@ -984,12 +984,12 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
@@ -999,17 +999,17 @@
       <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="30" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
       <c r="H10" s="6"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
@@ -1026,11 +1026,11 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
       <c r="H11" s="6"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
@@ -1049,11 +1049,11 @@
       <c r="D12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
       <c r="H12" s="7"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
@@ -1070,11 +1070,11 @@
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
       <c r="H13" s="6"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
@@ -1091,11 +1091,11 @@
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
       <c r="H14" s="6"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
@@ -1222,16 +1222,16 @@
       <c r="O20" s="18"/>
     </row>
     <row r="21" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
@@ -1241,86 +1241,86 @@
       <c r="O21" s="18"/>
     </row>
     <row r="22" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
     </row>
     <row r="23" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
     </row>
     <row r="25" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
     </row>
     <row r="26" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
     </row>
     <row r="27" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
     </row>
     <row r="28" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
@@ -1335,98 +1335,98 @@
       <c r="H30" s="11"/>
     </row>
     <row r="31" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="25"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="25"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
     </row>
     <row r="37" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
@@ -1480,17 +1480,17 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="19"/>
+      <c r="C45" s="20"/>
       <c r="D45" s="2"/>
       <c r="H45" s="2"/>
-      <c r="I45" s="19" t="s">
+      <c r="I45" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
@@ -1569,17 +1569,17 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
-      <c r="B54" s="19" t="s">
+      <c r="B54" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C54" s="19"/>
+      <c r="C54" s="20"/>
       <c r="D54" s="6"/>
       <c r="H54" s="6"/>
-      <c r="I54" s="19" t="s">
+      <c r="I54" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="J54" s="19"/>
-      <c r="K54" s="19"/>
+      <c r="J54" s="20"/>
+      <c r="K54" s="20"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="17"/>
@@ -1657,42 +1657,41 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="16"/>
-      <c r="B109" s="20" t="s">
+      <c r="B109" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C109" s="20"/>
-      <c r="D109" s="20"/>
-      <c r="E109" s="20"/>
-      <c r="F109" s="20"/>
-      <c r="G109" s="20"/>
-      <c r="H109" s="20"/>
-      <c r="I109" s="20"/>
-      <c r="J109" s="20"/>
-      <c r="K109" s="20"/>
-      <c r="L109" s="20"/>
-      <c r="M109" s="20"/>
+      <c r="C109" s="21"/>
+      <c r="D109" s="21"/>
+      <c r="E109" s="21"/>
+      <c r="F109" s="21"/>
+      <c r="G109" s="21"/>
+      <c r="H109" s="21"/>
+      <c r="I109" s="21"/>
+      <c r="J109" s="21"/>
+      <c r="K109" s="21"/>
+      <c r="L109" s="21"/>
+      <c r="M109" s="21"/>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="16"/>
-      <c r="B110" s="20"/>
-      <c r="C110" s="20"/>
-      <c r="D110" s="20"/>
-      <c r="E110" s="20"/>
-      <c r="F110" s="20"/>
-      <c r="G110" s="20"/>
-      <c r="H110" s="20"/>
-      <c r="I110" s="20"/>
-      <c r="J110" s="20"/>
-      <c r="K110" s="20"/>
-      <c r="L110" s="20"/>
-      <c r="M110" s="20"/>
+      <c r="B110" s="21"/>
+      <c r="C110" s="21"/>
+      <c r="D110" s="21"/>
+      <c r="E110" s="21"/>
+      <c r="F110" s="21"/>
+      <c r="G110" s="21"/>
+      <c r="H110" s="21"/>
+      <c r="I110" s="21"/>
+      <c r="J110" s="21"/>
+      <c r="K110" s="21"/>
+      <c r="L110" s="21"/>
+      <c r="M110" s="21"/>
     </row>
     <row r="220" spans="16:16" x14ac:dyDescent="0.3">
-      <c r="P220" s="32"/>
+      <c r="P220" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E13:G13"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="I45:K45"/>
@@ -1710,9 +1709,10 @@
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.51181102362204722" bottom="0.51181102362204722" header="0" footer="0.31496062992125984"/>
-  <pageSetup paperSize="3" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>